<commit_message>
changed the rack map
</commit_message>
<xml_diff>
--- a/Assay Experiment/Round1_chlarackmap.xlsx
+++ b/Assay Experiment/Round1_chlarackmap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c9f30cf11edfc58c/2023 Rtudio/Reservoirs_sulfate/Assay Experiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="205" documentId="8_{E79DB229-B890-412B-9399-02799287D236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F4D4E9A-7615-4351-90E6-3EAB26AABC41}"/>
+  <xr:revisionPtr revIDLastSave="211" documentId="8_{E79DB229-B890-412B-9399-02799287D236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B48BA99-F7C1-4EF4-8A4B-34C6AF93A82A}"/>
   <bookViews>
-    <workbookView xWindow="7848" yWindow="660" windowWidth="13308" windowHeight="13020" xr2:uid="{FC9DBA0A-CE17-4368-BF26-1BC64C3C4842}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{FC9DBA0A-CE17-4368-BF26-1BC64C3C4842}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
   <dimension ref="A1:Z42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated rack my with the ethanol blanks
</commit_message>
<xml_diff>
--- a/Assay Experiment/Round1_chlarackmap.xlsx
+++ b/Assay Experiment/Round1_chlarackmap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c9f30cf11edfc58c/2023 Rtudio/Reservoirs_sulfate/Assay Experiment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abreefpilz\Documents\GitHub\Reservoirs_sulfate\Assay Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="211" documentId="8_{E79DB229-B890-412B-9399-02799287D236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B48BA99-F7C1-4EF4-8A4B-34C6AF93A82A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B2DE37-D6B7-4C1A-A06B-43D3F91D79A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{FC9DBA0A-CE17-4368-BF26-1BC64C3C4842}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{FC9DBA0A-CE17-4368-BF26-1BC64C3C4842}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
   <si>
     <t>Date_processed</t>
   </si>
@@ -75,7 +73,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -469,21 +467,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA67E96-68DA-4F9A-A01A-E1DF971CC175}">
-  <dimension ref="A1:Z42"/>
+  <dimension ref="A1:Z45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="132" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.90234375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.76171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="14.1" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -523,7 +521,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26">
       <c r="A2" s="4">
         <v>45849</v>
       </c>
@@ -561,7 +559,7 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26">
       <c r="A3" s="1">
         <v>45849</v>
       </c>
@@ -578,7 +576,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26">
       <c r="A4" s="1">
         <v>45849</v>
       </c>
@@ -595,7 +593,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26">
       <c r="A5" s="1">
         <v>45849</v>
       </c>
@@ -612,7 +610,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26">
       <c r="A6" s="1">
         <v>45849</v>
       </c>
@@ -629,7 +627,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26">
       <c r="A7" s="1">
         <v>45849</v>
       </c>
@@ -646,151 +644,151 @@
         <v>470</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26">
       <c r="A8" s="1">
         <v>45849</v>
       </c>
       <c r="B8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="E8">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
       <c r="A9" s="1">
         <v>45849</v>
       </c>
       <c r="B9">
-        <v>14</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
       </c>
       <c r="E9">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
       <c r="A10" s="1">
         <v>45849</v>
       </c>
       <c r="B10">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>470</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26">
       <c r="A11" s="1">
         <v>45849</v>
       </c>
       <c r="B11">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C11">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D11">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <v>470</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26">
       <c r="A12" s="1">
         <v>45849</v>
       </c>
       <c r="B12">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13" s="1">
+        <v>45849</v>
+      </c>
+      <c r="B13">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>32</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14" s="1">
+        <v>45849</v>
+      </c>
+      <c r="B14">
         <v>20</v>
       </c>
-      <c r="C12">
+      <c r="C14">
         <v>19</v>
       </c>
-      <c r="D12">
+      <c r="D14">
         <v>3</v>
       </c>
-      <c r="E12">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B13">
+      <c r="E14">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B16">
         <v>2</v>
       </c>
-      <c r="C13">
+      <c r="C16">
         <v>13</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>31</v>
-      </c>
-      <c r="D14">
-        <v>7</v>
-      </c>
-      <c r="E14">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B15">
-        <v>4</v>
-      </c>
-      <c r="C15">
-        <v>34</v>
-      </c>
-      <c r="D15">
-        <v>7</v>
-      </c>
-      <c r="E15">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B16">
-        <v>5</v>
-      </c>
-      <c r="C16">
-        <v>18</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -799,290 +797,287 @@
         <v>470</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>45854</v>
       </c>
       <c r="B17">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C17">
+        <v>31</v>
+      </c>
+      <c r="D17">
+        <v>7</v>
+      </c>
+      <c r="E17">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>34</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20">
         <v>16</v>
       </c>
-      <c r="D17">
+      <c r="D20">
         <v>1</v>
       </c>
-      <c r="E17">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B18">
-        <v>7</v>
-      </c>
-      <c r="C18">
+      <c r="E20">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21">
         <v>17</v>
       </c>
-      <c r="D18">
+      <c r="D21">
         <v>1</v>
       </c>
-      <c r="E18">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B19">
+      <c r="E21">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B22">
         <v>8</v>
       </c>
-      <c r="C19">
+      <c r="C22">
         <v>33</v>
       </c>
-      <c r="D19">
-        <v>7</v>
-      </c>
-      <c r="E19">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B20">
+      <c r="D22">
+        <v>7</v>
+      </c>
+      <c r="E22">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B23">
         <v>9</v>
       </c>
-      <c r="C20">
-        <v>6</v>
-      </c>
-      <c r="D20">
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23">
         <v>0</v>
       </c>
-      <c r="E20">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B21">
+      <c r="E23">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B24">
         <v>10</v>
       </c>
-      <c r="C21">
+      <c r="C24">
         <v>12</v>
       </c>
-      <c r="D21">
+      <c r="D24">
         <v>0.5</v>
       </c>
-      <c r="E21">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B22">
+      <c r="E24">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B25">
         <v>11</v>
       </c>
-      <c r="C22">
+      <c r="C25">
         <v>27</v>
       </c>
-      <c r="D22">
+      <c r="D25">
         <v>5</v>
       </c>
-      <c r="E22">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B23">
+      <c r="E25">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B26">
         <v>12</v>
       </c>
-      <c r="C23">
+      <c r="C26">
         <v>24</v>
       </c>
-      <c r="D23">
+      <c r="D26">
         <v>3</v>
       </c>
-      <c r="E23">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B24">
+      <c r="E26">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B27">
         <v>13</v>
       </c>
-      <c r="C24">
+      <c r="C27">
         <v>20</v>
       </c>
-      <c r="D24">
+      <c r="D27">
         <v>3</v>
       </c>
-      <c r="E24">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B25">
+      <c r="E27">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B28">
         <v>14</v>
       </c>
-      <c r="C25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B26">
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B29">
         <v>15</v>
       </c>
-      <c r="C26">
+      <c r="C29">
         <v>9</v>
       </c>
-      <c r="D26">
+      <c r="D29">
         <v>0.5</v>
       </c>
-      <c r="E26">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B27">
+      <c r="E29">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B30">
         <v>16</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C30" t="s">
         <v>8</v>
       </c>
-      <c r="D27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27">
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30">
         <v>1000</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B28">
+    <row r="31" spans="1:5">
+      <c r="A31" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B31">
         <v>17</v>
       </c>
-      <c r="C28">
+      <c r="C31">
         <v>25</v>
       </c>
-      <c r="D28">
+      <c r="D31">
         <v>5</v>
       </c>
-      <c r="E28">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B29">
+      <c r="E31">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B32">
         <v>18</v>
       </c>
-      <c r="C29">
+      <c r="C32">
         <v>14</v>
       </c>
-      <c r="D29">
+      <c r="D32">
         <v>1</v>
       </c>
-      <c r="E29">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B30">
+      <c r="E32">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B33">
         <v>19</v>
       </c>
-      <c r="C30">
+      <c r="C33">
         <v>8</v>
-      </c>
-      <c r="D30">
-        <v>0.5</v>
-      </c>
-      <c r="E30">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B31">
-        <v>20</v>
-      </c>
-      <c r="C31">
-        <v>22</v>
-      </c>
-      <c r="D31">
-        <v>3</v>
-      </c>
-      <c r="E31">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B32">
-        <v>21</v>
-      </c>
-      <c r="C32">
-        <v>2</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>470</v>
-      </c>
-      <c r="F32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B33">
-        <v>22</v>
-      </c>
-      <c r="C33">
-        <v>10</v>
       </c>
       <c r="D33">
         <v>0.5</v>
@@ -1090,19 +1085,16 @@
       <c r="E33">
         <v>470</v>
       </c>
-      <c r="F33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="1">
         <v>45854</v>
       </c>
       <c r="B34">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C34">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D34">
         <v>3</v>
@@ -1111,83 +1103,89 @@
         <v>470</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6">
       <c r="A35" s="1">
         <v>45854</v>
       </c>
       <c r="B35">
+        <v>21</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>470</v>
+      </c>
+      <c r="F35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B36">
+        <v>22</v>
+      </c>
+      <c r="C36">
+        <v>10</v>
+      </c>
+      <c r="D36">
+        <v>0.5</v>
+      </c>
+      <c r="E36">
+        <v>470</v>
+      </c>
+      <c r="F36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B37">
+        <v>23</v>
+      </c>
+      <c r="C37">
+        <v>23</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B38">
         <v>24</v>
       </c>
-      <c r="C35">
+      <c r="C38">
         <v>28</v>
       </c>
-      <c r="D35">
+      <c r="D38">
         <v>5</v>
       </c>
-      <c r="E35">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B36">
+      <c r="E38">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B39">
         <v>25</v>
       </c>
-      <c r="C36">
+      <c r="C39">
         <v>30</v>
-      </c>
-      <c r="D36">
-        <v>5</v>
-      </c>
-      <c r="E36">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B37">
-        <v>26</v>
-      </c>
-      <c r="C37">
-        <v>5</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B38">
-        <v>27</v>
-      </c>
-      <c r="C38">
-        <v>36</v>
-      </c>
-      <c r="D38">
-        <v>7</v>
-      </c>
-      <c r="E38">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B39">
-        <v>28</v>
-      </c>
-      <c r="C39">
-        <v>26</v>
       </c>
       <c r="D39">
         <v>5</v>
@@ -1196,54 +1194,105 @@
         <v>470</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6">
       <c r="A40" s="1">
         <v>45854</v>
       </c>
       <c r="B40">
+        <v>26</v>
+      </c>
+      <c r="C40">
+        <v>5</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B41">
+        <v>27</v>
+      </c>
+      <c r="C41">
+        <v>36</v>
+      </c>
+      <c r="D41">
+        <v>7</v>
+      </c>
+      <c r="E41">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B42">
+        <v>28</v>
+      </c>
+      <c r="C42">
+        <v>26</v>
+      </c>
+      <c r="D42">
+        <v>5</v>
+      </c>
+      <c r="E42">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B43">
         <v>29</v>
       </c>
-      <c r="C40">
+      <c r="C43">
         <v>35</v>
       </c>
-      <c r="D40">
-        <v>7</v>
-      </c>
-      <c r="E40">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B41">
+      <c r="D43">
+        <v>7</v>
+      </c>
+      <c r="E43">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B44">
         <v>30</v>
       </c>
-      <c r="C41">
+      <c r="C44">
         <v>1</v>
       </c>
-      <c r="D41">
+      <c r="D44">
         <v>0</v>
       </c>
-      <c r="E41">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
-        <v>45854</v>
-      </c>
-      <c r="B42">
+      <c r="E44">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="1">
+        <v>45854</v>
+      </c>
+      <c r="B45">
         <v>31</v>
       </c>
-      <c r="C42" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" t="s">
-        <v>6</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added dose and Assay_num
</commit_message>
<xml_diff>
--- a/Assay Experiment/Round1_chlarackmap.xlsx
+++ b/Assay Experiment/Round1_chlarackmap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abreefpilz\Documents\GitHub\Reservoirs_sulfate\Assay Experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c9f30cf11edfc58c/2023 Rtudio/Reservoirs_sulfate/Assay Experiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B2DE37-D6B7-4C1A-A06B-43D3F91D79A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{C6B2DE37-D6B7-4C1A-A06B-43D3F91D79A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54D001BE-7994-4B57-BEF9-092687948DBF}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{FC9DBA0A-CE17-4368-BF26-1BC64C3C4842}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{FC9DBA0A-CE17-4368-BF26-1BC64C3C4842}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
   <si>
     <t>Date_processed</t>
   </si>
@@ -68,12 +68,18 @@
   <si>
     <t>Num_ID</t>
   </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Assay_num</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,10 +150,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -469,19 +471,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA67E96-68DA-4F9A-A01A-E1DF971CC175}">
   <dimension ref="A1:Z45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="132" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.90234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.76171875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.1" thickBot="1">
+    <row r="1" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -500,8 +503,12 @@
       <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -521,7 +528,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>45849</v>
       </c>
@@ -539,7 +546,9 @@
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -559,7 +568,7 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>45849</v>
       </c>
@@ -575,8 +584,11 @@
       <c r="E3">
         <v>470</v>
       </c>
-    </row>
-    <row r="4" spans="1:26">
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>45849</v>
       </c>
@@ -592,8 +604,11 @@
       <c r="E4">
         <v>470</v>
       </c>
-    </row>
-    <row r="5" spans="1:26">
+      <c r="H4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45849</v>
       </c>
@@ -609,8 +624,11 @@
       <c r="E5">
         <v>470</v>
       </c>
-    </row>
-    <row r="6" spans="1:26">
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>45849</v>
       </c>
@@ -626,8 +644,11 @@
       <c r="E6">
         <v>470</v>
       </c>
-    </row>
-    <row r="7" spans="1:26">
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>45849</v>
       </c>
@@ -643,8 +664,11 @@
       <c r="E7">
         <v>470</v>
       </c>
-    </row>
-    <row r="8" spans="1:26">
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>45849</v>
       </c>
@@ -660,8 +684,11 @@
       <c r="E8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:26">
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>45849</v>
       </c>
@@ -677,8 +704,11 @@
       <c r="E9">
         <v>1000</v>
       </c>
-    </row>
-    <row r="10" spans="1:26">
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>45849</v>
       </c>
@@ -694,8 +724,11 @@
       <c r="E10">
         <v>470</v>
       </c>
-    </row>
-    <row r="11" spans="1:26">
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>45849</v>
       </c>
@@ -711,8 +744,11 @@
       <c r="E11">
         <v>470</v>
       </c>
-    </row>
-    <row r="12" spans="1:26">
+      <c r="H11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>45849</v>
       </c>
@@ -728,8 +764,11 @@
       <c r="E12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:26">
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>45849</v>
       </c>
@@ -745,8 +784,11 @@
       <c r="E13">
         <v>470</v>
       </c>
-    </row>
-    <row r="14" spans="1:26">
+      <c r="H13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>45849</v>
       </c>
@@ -762,8 +804,11 @@
       <c r="E14">
         <v>470</v>
       </c>
-    </row>
-    <row r="15" spans="1:26">
+      <c r="H14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>45854</v>
       </c>
@@ -779,8 +824,11 @@
       <c r="E15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:26">
+      <c r="H15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>45854</v>
       </c>
@@ -796,8 +844,11 @@
       <c r="E16">
         <v>470</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="H16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>45854</v>
       </c>
@@ -813,8 +864,11 @@
       <c r="E17">
         <v>470</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="H17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>45854</v>
       </c>
@@ -830,8 +884,11 @@
       <c r="E18">
         <v>470</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="H18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>45854</v>
       </c>
@@ -847,8 +904,11 @@
       <c r="E19">
         <v>470</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="H19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>45854</v>
       </c>
@@ -864,8 +924,11 @@
       <c r="E20">
         <v>470</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="H20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>45854</v>
       </c>
@@ -881,8 +944,11 @@
       <c r="E21">
         <v>470</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="H21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>45854</v>
       </c>
@@ -898,8 +964,11 @@
       <c r="E22">
         <v>470</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="H22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>45854</v>
       </c>
@@ -915,8 +984,11 @@
       <c r="E23">
         <v>470</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="H23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>45854</v>
       </c>
@@ -932,8 +1004,11 @@
       <c r="E24">
         <v>470</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="H24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>45854</v>
       </c>
@@ -949,8 +1024,11 @@
       <c r="E25">
         <v>470</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="H25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>45854</v>
       </c>
@@ -966,8 +1044,11 @@
       <c r="E26">
         <v>470</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="H26" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>45854</v>
       </c>
@@ -983,8 +1064,11 @@
       <c r="E27">
         <v>470</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="H27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>45854</v>
       </c>
@@ -1000,8 +1084,11 @@
       <c r="E28" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="H28" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>45854</v>
       </c>
@@ -1017,8 +1104,11 @@
       <c r="E29">
         <v>470</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="H29" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>45854</v>
       </c>
@@ -1034,8 +1124,11 @@
       <c r="E30">
         <v>1000</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="H30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>45854</v>
       </c>
@@ -1051,8 +1144,11 @@
       <c r="E31">
         <v>470</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="H31" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>45854</v>
       </c>
@@ -1068,8 +1164,11 @@
       <c r="E32">
         <v>470</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="H32" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>45854</v>
       </c>
@@ -1085,8 +1184,11 @@
       <c r="E33">
         <v>470</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="H33" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>45854</v>
       </c>
@@ -1102,8 +1204,11 @@
       <c r="E34">
         <v>470</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="H34" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>45854</v>
       </c>
@@ -1122,8 +1227,11 @@
       <c r="F35" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="H35" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>45854</v>
       </c>
@@ -1142,8 +1250,11 @@
       <c r="F36" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="H36" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>45854</v>
       </c>
@@ -1159,8 +1270,11 @@
       <c r="E37">
         <v>470</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="H37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>45854</v>
       </c>
@@ -1176,8 +1290,11 @@
       <c r="E38">
         <v>470</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="H38" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>45854</v>
       </c>
@@ -1193,8 +1310,11 @@
       <c r="E39">
         <v>470</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="H39" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>45854</v>
       </c>
@@ -1210,8 +1330,11 @@
       <c r="E40">
         <v>470</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="H40" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>45854</v>
       </c>
@@ -1227,8 +1350,11 @@
       <c r="E41">
         <v>470</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="H41" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>45854</v>
       </c>
@@ -1244,8 +1370,11 @@
       <c r="E42">
         <v>470</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="H42" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>45854</v>
       </c>
@@ -1261,8 +1390,11 @@
       <c r="E43">
         <v>470</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="H43" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>45854</v>
       </c>
@@ -1278,8 +1410,11 @@
       <c r="E44">
         <v>470</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="H44" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>45854</v>
       </c>
@@ -1295,9 +1430,13 @@
       <c r="E45" t="s">
         <v>6</v>
       </c>
+      <c r="H45" s="3">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <cellWatches>
     <cellWatch r="A1"/>
     <cellWatch r="B1"/>
@@ -1305,6 +1444,8 @@
     <cellWatch r="D1"/>
     <cellWatch r="E1"/>
     <cellWatch r="F1"/>
+    <cellWatch r="G1"/>
+    <cellWatch r="H1"/>
   </cellWatches>
 </worksheet>
 </file>
</xml_diff>